<commit_message>
all to average changes
</commit_message>
<xml_diff>
--- a/data/food_carbon_footprint_data.xlsx
+++ b/data/food_carbon_footprint_data.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlatimer\Documents\personal\EDLD MS\EDLD 652 DS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlatimer\Documents\personal\EDLD MS\EDLD 652 DS\Project\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="158">
   <si>
     <t>Argentina</t>
   </si>
@@ -529,9 +529,6 @@
   </si>
   <si>
     <t>ranking</t>
-  </si>
-  <si>
-    <t>all</t>
   </si>
   <si>
     <t>average</t>
@@ -1944,8 +1941,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q132"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" topLeftCell="A127" workbookViewId="0">
+      <selection activeCell="B133" sqref="B133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8502,38 +8499,38 @@
       </c>
     </row>
     <row r="132" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A132" t="s">
-        <v>158</v>
+      <c r="A132">
+        <v>0</v>
       </c>
       <c r="B132" s="2" t="s">
         <v>157</v>
       </c>
       <c r="C132" s="118">
-        <f>AVERAGE(C2:C131)</f>
+        <f t="shared" ref="C132:I132" si="0">AVERAGE(C2:C131)</f>
         <v>57.070076923076911</v>
       </c>
       <c r="D132" s="118">
-        <f>AVERAGE(D2:D131)</f>
+        <f t="shared" si="0"/>
         <v>22.793538461538461</v>
       </c>
       <c r="E132" s="118">
-        <f>AVERAGE(E2:E131)</f>
+        <f t="shared" si="0"/>
         <v>374.10199999999986</v>
       </c>
       <c r="F132" s="118">
-        <f>AVERAGE(F2:F131)</f>
+        <f t="shared" si="0"/>
         <v>91.056769230769234</v>
       </c>
       <c r="G132" s="118">
-        <f>AVERAGE(G2:G131)</f>
+        <f t="shared" si="0"/>
         <v>27.601692307692311</v>
       </c>
       <c r="H132" s="118">
-        <f>AVERAGE(H2:H131)</f>
+        <f t="shared" si="0"/>
         <v>7.4996153846153817</v>
       </c>
       <c r="I132" s="118">
-        <f>AVERAGE(I2:I131)</f>
+        <f t="shared" si="0"/>
         <v>179.15384615384613</v>
       </c>
       <c r="J132" s="118">
@@ -8545,15 +8542,15 @@
         <v>13.644461538461533</v>
       </c>
       <c r="L132" s="118">
-        <f t="shared" ref="L132:O132" si="0">AVERAGE(L2:L131)</f>
+        <f t="shared" ref="L132:N132" si="1">AVERAGE(L2:L131)</f>
         <v>37.591615384615373</v>
       </c>
       <c r="M132" s="118">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.38730769230769241</v>
       </c>
       <c r="N132" s="118">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.3229999999999986</v>
       </c>
       <c r="O132" s="118">

</xml_diff>